<commit_message>
Updated template and test file
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40480" yWindow="3040" windowWidth="27920" windowHeight="18100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>SAFE Project ID</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Keywords</t>
+  </si>
+  <si>
+    <t>Class</t>
   </si>
 </sst>
 </file>
@@ -675,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -815,22 +818,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -844,80 +847,91 @@
         <v>6</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1"/>
-    <row r="3" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1"/>
-    <row r="4" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+    <row r="2" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1"/>
+    <row r="3" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1"/>
+    <row r="4" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
-      <c r="I10" s="7"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1"/>
-    <row r="12" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1"/>
-    <row r="13" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="J10" s="7"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1"/>
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1"/>
+    <row r="13" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="G13" s="7"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1"/>
-    <row r="16" spans="1:11" s="6" customFormat="1" ht="17" customHeight="1"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1"/>
+    <row r="16" spans="1:12" s="6" customFormat="1" ht="17" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated Test and Template Excel files, some auxilliary testing and exploration files
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>SAFE Project ID</t>
   </si>
@@ -117,23 +117,45 @@
     <t>interaction_name</t>
   </si>
   <si>
-    <t>Scientific name</t>
-  </si>
-  <si>
     <t>Parent name</t>
   </si>
   <si>
     <t>Parent type</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Taxon ID</t>
+  </si>
+  <si>
+    <t>Parent ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,8 +187,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -175,7 +201,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -641,7 +671,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -653,28 +683,33 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>